<commit_message>
Move chart to separate modal page AddRow functionality in DataService Add Message to ViewModelBase Move IsRefreshing to ViewModelBase Update Excelfile to use new chart type and to auto update pivot table on open
</commit_message>
<xml_diff>
--- a/src/ExcelFormsTest/ExcelFormsTest/ExcelFormsTest/Resources/Expenses.xlsx
+++ b/src/ExcelFormsTest/ExcelFormsTest/ExcelFormsTest/Resources/Expenses.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Vendor</t>
   </si>
@@ -47,21 +47,6 @@
   </si>
   <si>
     <t>Sum of Amount</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -149,13 +134,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -181,13 +172,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -203,36 +200,7 @@
         <c:idx val="0"/>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
+        <c:idx val="1"/>
         <c:dLbl>
           <c:idx val="0"/>
           <c:dLblPos val="inEnd"/>
@@ -248,32 +216,99 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="3"/>
+        <c:idx val="2"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent6">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent6">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="diamond"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -291,24 +326,99 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:delete val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -345,7 +455,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="65"/>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
         <c:axId val="406334384"/>
         <c:axId val="406334056"/>
       </c:barChart>
@@ -355,18 +466,18 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -378,11 +489,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -406,28 +516,16 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="95000"/>
-                      <a:lumOff val="5000"/>
-                      <a:alpha val="42000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                      <a:alpha val="36000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -449,42 +547,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -493,30 +555,25 @@
     <a:gradFill flip="none" rotWithShape="1">
       <a:gsLst>
         <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
         </a:gs>
         <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
           </a:schemeClr>
         </a:gs>
       </a:gsLst>
       <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
       </a:path>
       <a:tileRect/>
     </a:gradFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -541,7 +598,6 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -561,41 +617,39 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea>
     <cs:lnRef idx="0"/>
@@ -608,160 +662,124 @@
       <a:gradFill flip="none" rotWithShape="1">
         <a:gsLst>
           <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="39000">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
           </a:gs>
           <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="75000"/>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
             </a:schemeClr>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
         <a:tileRect/>
       </a:gradFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -777,17 +795,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -799,20 +816,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -823,14 +840,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -842,14 +859,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -861,7 +877,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -869,28 +885,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -900,28 +904,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -930,14 +922,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -949,14 +941,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -967,19 +959,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-          <a:alpha val="39000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea>
@@ -987,7 +970,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -995,7 +978,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1003,17 +986,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1026,14 +1008,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1045,12 +1027,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1059,7 +1048,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -1074,9 +1063,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1086,7 +1074,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1094,9 +1082,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1107,16 +1095,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1124,7 +1106,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -1166,9 +1148,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="42531.657463541669" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Author" refreshedDate="42531.657463541669" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
-    <worksheetSource name="Table1"/>
+    <worksheetSource name="Table1" r:id="rId2"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="Vendor" numFmtId="0">
@@ -1209,7 +1191,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1243,7 +1225,7 @@
     <dataField name="Sum of Amount" fld="2" baseField="1" baseItem="2" numFmtId="164"/>
   </dataFields>
   <chartFormats count="1">
-    <chartFormat chart="0" format="3" series="1">
+    <chartFormat chart="0" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1574,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1610,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>